<commit_message>
feat(backend): enhance job processing with improved error handling and add run with job_id endpoint
</commit_message>
<xml_diff>
--- a/backend/test/fixtures/upload/valid_xlsx.xlsx
+++ b/backend/test/fixtures/upload/valid_xlsx.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larrywang/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larrywang/media-metrics-lab/backend/test/fixtures/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C137BB2-0FCC-4D4B-A5D2-A033C90BCAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B629482E-7DF1-1C4A-A7FC-664BF626B786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4040" yWindow="2080" windowWidth="27920" windowHeight="17440" xr2:uid="{BDFBCB01-7B13-9946-8AEC-DC10BFD43DE8}"/>
+    <workbookView xWindow="1100" yWindow="2080" windowWidth="27920" windowHeight="17440" xr2:uid="{BDFBCB01-7B13-9946-8AEC-DC10BFD43DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="valid_csv" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>platform</t>
   </si>
@@ -54,6 +54,12 @@
   </si>
   <si>
     <t>tiktok</t>
+  </si>
+  <si>
+    <t>instagram</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/pine</t>
   </si>
 </sst>
 </file>
@@ -436,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1C1C22-1250-8F4B-815B-FB7B5E8809EF}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -471,10 +477,19 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{8FE4E010-7386-7340-A0A8-51A839179466}"/>
     <hyperlink ref="B3" r:id="rId2" xr:uid="{CC4A490E-D355-BC43-BCD3-8FF8017DE782}"/>
+    <hyperlink ref="B4" r:id="rId3" xr:uid="{66CBC72E-B691-6745-903E-05A968AE812E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: implement YouTube fetcher with yt-dlp integration and update environment configuration
</commit_message>
<xml_diff>
--- a/backend/test/fixtures/upload/valid_xlsx.xlsx
+++ b/backend/test/fixtures/upload/valid_xlsx.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larrywang/media-metrics-lab/backend/test/fixtures/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B629482E-7DF1-1C4A-A7FC-664BF626B786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EF85A8-74E7-E74D-90B5-41487BA19E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1100" yWindow="2080" windowWidth="27920" windowHeight="17440" xr2:uid="{BDFBCB01-7B13-9946-8AEC-DC10BFD43DE8}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>platform</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>https://www.instagram.com/pine</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=whCINxitNkM</t>
   </si>
 </sst>
 </file>
@@ -442,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1C1C22-1250-8F4B-815B-FB7B5E8809EF}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,6 +488,14 @@
         <v>7</v>
       </c>
     </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{8FE4E010-7386-7340-A0A8-51A839179466}"/>

</xml_diff>

<commit_message>
feat: add metadata endpoint and enhance JobDetailPage with YouTube fetcher info visually. Closes issue #17
</commit_message>
<xml_diff>
--- a/backend/test/fixtures/upload/valid_xlsx.xlsx
+++ b/backend/test/fixtures/upload/valid_xlsx.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/larrywang/media-metrics-lab/backend/test/fixtures/upload/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EF85A8-74E7-E74D-90B5-41487BA19E5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AAACA6-F894-B44E-AA43-595F39F4380B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1100" yWindow="2080" windowWidth="27920" windowHeight="17440" xr2:uid="{BDFBCB01-7B13-9946-8AEC-DC10BFD43DE8}"/>
+    <workbookView xWindow="-400" yWindow="6900" windowWidth="27920" windowHeight="17440" xr2:uid="{BDFBCB01-7B13-9946-8AEC-DC10BFD43DE8}"/>
   </bookViews>
   <sheets>
     <sheet name="valid_csv" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="15">
   <si>
     <t>platform</t>
   </si>
@@ -63,6 +63,24 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=whCINxitNkM</t>
+  </si>
+  <si>
+    <t>https://youtu.be/fDJ2NrRRoB8?si=8Jpe-jjjUCR0Vd2m</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=jcb6Lygf3LQ</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=W69ZXgHm65A&amp;list=RDW69ZXgHm65A&amp;start_radio=1</t>
+  </si>
+  <si>
+    <t>https://www.tiktok.com/@paramountpics/video/7551460293851811103</t>
+  </si>
+  <si>
+    <t>https://www.tiktok.com/@aleko.so/video/7556646272849956107</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/shorts/5LekKnvD83E</t>
   </si>
 </sst>
 </file>
@@ -445,10 +463,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D1C1C22-1250-8F4B-815B-FB7B5E8809EF}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,6 +514,54 @@
         <v>8</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{8FE4E010-7386-7340-A0A8-51A839179466}"/>

</xml_diff>